<commit_message>
Updated the test scenario doc
Copy originally uploaded was not final it was also missing a Legend
</commit_message>
<xml_diff>
--- a/doc/Test_Scenario_doc.xlsx
+++ b/doc/Test_Scenario_doc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\cabinet\work$\mtm464\cmpt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingmack1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="114">
   <si>
     <t>Project Name</t>
   </si>
@@ -328,6 +328,51 @@
   </si>
   <si>
     <t>REQ_25</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>UC</t>
+  </si>
+  <si>
+    <t>SYS</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FT </t>
+  </si>
+  <si>
+    <t>UX</t>
+  </si>
+  <si>
+    <t>Test Scenarios</t>
+  </si>
+  <si>
+    <t>Test cases</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>System test</t>
+  </si>
+  <si>
+    <t>Feature test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Acceptance </t>
+  </si>
+  <si>
+    <t>Integration test</t>
   </si>
 </sst>
 </file>
@@ -444,7 +489,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -504,11 +549,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -529,23 +583,18 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,13 +611,26 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -578,20 +640,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -952,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D6"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,22 +1024,24 @@
     <col min="9" max="9" width="26.42578125" customWidth="1"/>
     <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.42578125" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="29"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
@@ -990,7 +1049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1011,320 +1070,381 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
       <c r="J3" s="6"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="30" t="s">
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="25" t="s">
+      <c r="K5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="25"/>
+      <c r="L5" s="30"/>
       <c r="M5" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O5" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="P5" s="44"/>
+    </row>
+    <row r="6" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
       <c r="J6" s="11"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
       <c r="M6" s="11"/>
-    </row>
-    <row r="7" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
       <c r="J7" s="11"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
       <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
       <c r="M8" s="11"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O8" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
       <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="23"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
       <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="23"/>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
+      <c r="K11" s="33"/>
+      <c r="L11" s="33"/>
       <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O11" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="P11" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="12"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
       <c r="M12" s="12"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O12" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="P12" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="12"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="12"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
       <c r="M14" s="12"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
+      <c r="K15" s="34"/>
+      <c r="L15" s="34"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="15"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="21"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="35"/>
       <c r="M18" s="2"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="35"/>
       <c r="M19" s="2"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
       <c r="M20" s="2"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B13:D13"/>
+  <mergeCells count="51">
+    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E15:I15"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="B15:D15"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B9:D9"/>
@@ -1341,32 +1461,18 @@
     <mergeCell ref="E14:I14"/>
     <mergeCell ref="E12:I12"/>
     <mergeCell ref="E13:I13"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E15:I15"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="E19:I19"/>
-    <mergeCell ref="E20:I20"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:XFD20">
+  <conditionalFormatting sqref="A6:XFD20 A5:O5 Q5:XFD5">
     <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>IFCOUNT($A$6,"TS_UC_*")</formula>
     </cfRule>
@@ -1386,215 +1492,215 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" style="39" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="20" customWidth="1"/>
     <col min="3" max="3" width="71.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="21" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="22" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="22" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="22" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="22" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="22" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="22" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="22" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="22" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="22" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="22" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="22" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="22" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="22" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="22" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="22" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="22" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="22" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="s">
+      <c r="B26" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="22" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" s="43" t="s">
+      <c r="B27" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="22" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1620,17 +1726,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
       <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1639,144 +1745,144 @@
       <c r="B2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="13"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37" t="s">
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1787,168 +1893,160 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="19"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
       <c r="I12" s="14"/>
       <c r="J12" s="17"/>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="B22" s="42"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="ssMck9pFw9V9ldaRh95JdUDD8wnLuOhg1UYMLEQiEEfnWR0/8Jw9q1OIkPMKZMdwoXtYmetBhN0HFkcJg6QjIw==" saltValue="1N/vuZnn8YFXm0mmZjxkEA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="35">
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H2:J2"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="C6:J7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="C21:J23"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
     <mergeCell ref="F17:H17"/>
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="C12:E12"/>
@@ -1962,13 +2060,21 @@
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="F16:H16"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="C21:J23"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="C6:J7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C8:J10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1985,17 +2091,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2004,144 +2110,144 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="18" t="s">
         <v>44</v>
       </c>
@@ -2152,152 +2258,177 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="14"/>
       <c r="J21" s="17"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:B24"/>
@@ -2308,31 +2439,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:J8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:J11"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2349,17 +2455,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2368,144 +2474,144 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="18" t="s">
         <v>44</v>
       </c>
@@ -2516,152 +2622,177 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="14"/>
       <c r="J21" s="17"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:B24"/>
@@ -2672,31 +2803,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:J8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:J11"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2713,17 +2819,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
@@ -2732,144 +2838,144 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="18" t="s">
         <v>44</v>
       </c>
@@ -2880,152 +2986,177 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="14"/>
       <c r="J21" s="17"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:B24"/>
@@ -3036,31 +3167,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:J8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:J11"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3077,17 +3183,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
@@ -3096,144 +3202,144 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="18" t="s">
         <v>44</v>
       </c>
@@ -3244,152 +3350,177 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="14"/>
       <c r="J21" s="17"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:B24"/>
@@ -3400,31 +3531,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:J8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:J11"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3441,17 +3547,17 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1" t="s">
         <v>14</v>
       </c>
@@ -3460,144 +3566,144 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="13"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
       <c r="K4" s="13"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
-      <c r="J5" s="38"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
       <c r="K5" s="13"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38"/>
-      <c r="J6" s="38"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="35"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
       <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
       <c r="K11" s="13"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37" t="s">
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
       <c r="I12" s="18" t="s">
         <v>44</v>
       </c>
@@ -3608,152 +3714,177 @@
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="19"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
       <c r="I13" s="14"/>
       <c r="J13" s="17"/>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="19"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="31"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
       <c r="I14" s="14"/>
       <c r="J14" s="17"/>
       <c r="K14" s="13"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="19"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="31"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
       <c r="I15" s="14"/>
       <c r="J15" s="17"/>
       <c r="K15" s="13"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="19"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
       <c r="I16" s="14"/>
       <c r="J16" s="17"/>
       <c r="K16" s="13"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="19"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
       <c r="I17" s="14"/>
       <c r="J17" s="17"/>
       <c r="K17" s="13"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="19"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="41"/>
+      <c r="H18" s="41"/>
       <c r="I18" s="14"/>
       <c r="J18" s="17"/>
       <c r="K18" s="13"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="19"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
       <c r="I19" s="14"/>
       <c r="J19" s="17"/>
       <c r="K19" s="13"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
       <c r="I20" s="14"/>
       <c r="J20" s="17"/>
       <c r="K20" s="13"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="31"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
       <c r="I21" s="14"/>
       <c r="J21" s="17"/>
       <c r="K21" s="13"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
       <c r="K22" s="13"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
       <c r="K23" s="13"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="32"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:J8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:J11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="F15:H15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="F17:H17"/>
     <mergeCell ref="C21:E21"/>
     <mergeCell ref="F21:H21"/>
     <mergeCell ref="B22:B24"/>
@@ -3764,31 +3895,6 @@
     <mergeCell ref="F19:H19"/>
     <mergeCell ref="C20:E20"/>
     <mergeCell ref="F20:H20"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="F16:H16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:J8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:J11"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="H5:J5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>